<commit_message>
added test de perception
</commit_message>
<xml_diff>
--- a/docs/gestion de projet/milestone 1/management/tests de perception/inessa kechek.xlsx
+++ b/docs/gestion de projet/milestone 1/management/tests de perception/inessa kechek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Downloads\projet-iot\hardware-sensor\docs\gestion de projet\milestone 1\management\tests de perception\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iness\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523EFF10-55D5-4220-B859-CCA6ECFF9F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFC79DE-2958-4DC0-A09A-4C4D5F1817F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="34776" windowHeight="21096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaire" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -237,9 +235,6 @@
     <t>J'ai tendance à m'ennuyer si je ne me trouve pas avec des personnes suffisament impliquées et dynamiques</t>
   </si>
   <si>
-    <t>Je n'arrive pas toujours à expliquer certains aspects conplexes d'un sujet</t>
-  </si>
-  <si>
     <t>J'ai conscience de demander aux autres des choses que je n'arriverais pas à faire moi-même</t>
   </si>
   <si>
@@ -813,6 +808,9 @@
   </si>
   <si>
     <t>En dépit des pressions conflictuelles, je poursuivrai mes efforts pour faire avancer ce qui doit être réalisé</t>
+  </si>
+  <si>
+    <t>Je n'arrive pas toujours à expliquer certains aspects complexes d'un sujet</t>
   </si>
 </sst>
 </file>
@@ -1463,11 +1461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A70" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="68.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" style="3"/>
@@ -1475,13 +1473,13 @@
   <sheetData>
     <row r="2" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="B2" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:3" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1490,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>1</v>
@@ -1501,7 +1499,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1512,7 +1510,9 @@
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -1528,18 +1528,22 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" s="6"/>
+        <v>113</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>114</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -1605,16 +1609,20 @@
       <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" s="6"/>
+        <v>115</v>
+      </c>
+      <c r="C20" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
@@ -1623,14 +1631,16 @@
       <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22" s="6"/>
     </row>
@@ -1648,7 +1658,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="6"/>
     </row>
@@ -1698,14 +1708,16 @@
       <c r="B30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" s="6"/>
     </row>
@@ -1743,7 +1755,9 @@
       <c r="B35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="6"/>
+      <c r="C35" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
@@ -1761,7 +1775,9 @@
       <c r="B37" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="9"/>
+      <c r="C37" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1780,7 +1796,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C40" s="6"/>
     </row>
@@ -1789,9 +1805,11 @@
         <v>3</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" s="6"/>
+        <v>120</v>
+      </c>
+      <c r="C41" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
@@ -1836,7 +1854,9 @@
       <c r="B46" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="6"/>
+      <c r="C46" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
@@ -1852,9 +1872,11 @@
         <v>12</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="9"/>
+        <v>121</v>
+      </c>
+      <c r="C48" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1882,9 +1904,11 @@
         <v>3</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C52" s="6"/>
+        <v>122</v>
+      </c>
+      <c r="C52" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
@@ -1893,7 +1917,9 @@
       <c r="B53" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C53" s="6"/>
+      <c r="C53" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
@@ -1913,7 +1939,7 @@
       </c>
       <c r="C55" s="6"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>9</v>
       </c>
@@ -1927,9 +1953,11 @@
         <v>10</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C57" s="6"/>
+        <v>123</v>
+      </c>
+      <c r="C57" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
@@ -1945,7 +1973,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C59" s="9"/>
     </row>
@@ -2004,14 +2032,16 @@
       <c r="B66" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C66" s="6"/>
-    </row>
-    <row r="67" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C67" s="6"/>
     </row>
@@ -2020,9 +2050,11 @@
         <v>10</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C68" s="6"/>
+        <v>125</v>
+      </c>
+      <c r="C68" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="69" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
@@ -2040,7 +2072,9 @@
       <c r="B70" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C70" s="9"/>
+      <c r="C70" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="71" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -2079,7 +2113,9 @@
       <c r="B75" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C75" s="6"/>
+      <c r="C75" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="76" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
@@ -2088,14 +2124,16 @@
       <c r="B76" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C76" s="6"/>
+      <c r="C76" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C77" s="6"/>
     </row>
@@ -2104,7 +2142,7 @@
         <v>9</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="C78" s="6"/>
     </row>
@@ -2113,16 +2151,18 @@
         <v>10</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C79" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="C79" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="80" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C80" s="6"/>
     </row>
@@ -2131,7 +2171,7 @@
         <v>12</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C81" s="9"/>
     </row>
@@ -2145,11 +2185,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
       <selection activeCell="B36" sqref="B36:B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.109375" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" style="21" customWidth="1"/>
@@ -2158,10 +2198,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2171,13 +2211,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="26"/>
       <c r="C5" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2186,7 +2226,7 @@
         <v>Rôle complexe</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2196,13 +2236,13 @@
         <v>0</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="26"/>
       <c r="C9" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2211,57 +2251,57 @@
         <v>Rôle complexe</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="25">
         <f>Questionnaire!C12+Questionnaire!C20+Questionnaire!C34+Questionnaire!C41+Questionnaire!C59+Questionnaire!C62+Questionnaire!C80</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="26"/>
       <c r="C13" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="20" t="str">
         <f>IF(B12&gt;=16,"Rôle favori",IF(B12&gt;=10,"Rôle classique",IF(B12&gt;=6,"Rôle mineur",IF(B12&gt;=0,"Rôle complexe","false"))))</f>
-        <v>Rôle complexe</v>
+        <v>Rôle mineur</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="25">
         <f>Questionnaire!C14+Questionnaire!C18+Questionnaire!C37+Questionnaire!C44+Questionnaire!C52+Questionnaire!C68+Questionnaire!C77</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
       <c r="C17" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="20" t="str">
         <f>IF(B16&gt;=16,"Rôle favori",IF(B16&gt;=10,"Rôle classique",IF(B16&gt;=6,"Rôle mineur",IF(B16&gt;=0,"Rôle complexe","false"))))</f>
-        <v>Rôle complexe</v>
+        <v>Rôle classique</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2271,13 +2311,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="26"/>
       <c r="C21" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2286,144 +2326,144 @@
         <v>Rôle complexe</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="25">
         <f>Questionnaire!C11+Questionnaire!C26+Questionnaire!C30+Questionnaire!C46+Questionnaire!C57+Questionnaire!C66+Questionnaire!C75</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="26"/>
       <c r="C25" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="20" t="str">
         <f>IF(B24&gt;=16,"Rôle favori",IF(B24&gt;=10,"Rôle classique",IF(B24&gt;=6,"Rôle mineur",IF(B24&gt;=0,"Rôle complexe","false"))))</f>
-        <v>Rôle complexe</v>
+        <v>Rôle favori</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="25">
         <f>Questionnaire!C10+Questionnaire!C19+Questionnaire!C29+Questionnaire!C48+Questionnaire!C58+Questionnaire!C65+Questionnaire!C79</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="26"/>
       <c r="C29" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="20" t="str">
         <f>IF(B28&gt;=16,"Rôle favori",IF(B28&gt;=10,"Rôle classique",IF(B28&gt;=6,"Rôle mineur",IF(B28&gt;=0,"Rôle complexe","false"))))</f>
-        <v>Rôle complexe</v>
+        <v>Rôle classique</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="25">
         <f>Questionnaire!C7+Questionnaire!C21+Questionnaire!C35+Questionnaire!C47+Questionnaire!C55+Questionnaire!C70+Questionnaire!C76</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B33" s="26"/>
       <c r="C33" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="20" t="str">
         <f>IF(B32&gt;=16,"Rôle favori",IF(B32&gt;=10,"Rôle classique",IF(B32&gt;=6,"Rôle mineur",IF(B32&gt;=0,"Rôle complexe","false"))))</f>
-        <v>Rôle complexe</v>
+        <v>Rôle classique</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="25">
         <f>Questionnaire!C8+Questionnaire!C24+Questionnaire!C33+Questionnaire!C40+Questionnaire!C53+Questionnaire!C64+Questionnaire!C81</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B37" s="26"/>
       <c r="C37" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="20" t="str">
         <f>IF(B36&gt;=16,"Rôle favori",IF(B36&gt;=10,"Rôle classique",IF(B36&gt;=6,"Rôle mineur",IF(B36&gt;=0,"Rôle complexe","false"))))</f>
-        <v>Rôle complexe</v>
+        <v>Rôle mineur</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>